<commit_message>
webscrape progress: code set up, error handling, first two batches
</commit_message>
<xml_diff>
--- a/FLS_search_terms.XLSX
+++ b/FLS_search_terms.XLSX
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258AAD26-DDA7-431F-83AC-2912899EC657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Hip Fracture Service</t>
   </si>
@@ -28,9 +29,6 @@
     <t>Bone Health Program</t>
   </si>
   <si>
-    <t>Fracture Liaison Service</t>
-  </si>
-  <si>
     <t>Osteoporosis Clinic</t>
   </si>
   <si>
@@ -52,79 +50,109 @@
     <t>Geriatric Fracture Program</t>
   </si>
   <si>
-    <t>Geriatric Fracture Care Program</t>
-  </si>
-  <si>
-    <t>"Capture the Fracture" [US only]</t>
-  </si>
-  <si>
-    <t>Fracture Program/Center</t>
-  </si>
-  <si>
     <t>Fracture Service</t>
   </si>
   <si>
-    <t>Fracture Prevention Clinic/Program/Service/Center</t>
-  </si>
-  <si>
-    <t>Secondary Fracture Prevention Service/Center</t>
-  </si>
-  <si>
-    <t>Secondary Fracture Prevention Program (SFP)</t>
-  </si>
-  <si>
-    <t>Fragility Fracture Program</t>
-  </si>
-  <si>
     <t>Post Fracture Care Program</t>
   </si>
   <si>
-    <t>Post Fracture Care Services (PFC)</t>
-  </si>
-  <si>
     <t>Post Fracture Care Coordination Program</t>
   </si>
   <si>
     <t>Orthogeriatric Program</t>
   </si>
   <si>
-    <t>Orthogeriatric Service (OGS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osteoporosis Liaison Program </t>
-  </si>
-  <si>
-    <t>Osteoporosis Liaison Service (OLS)</t>
-  </si>
-  <si>
-    <t>"Healthy Bones Program"</t>
-  </si>
-  <si>
-    <t>Osteoporosis Prevention Center/Clinic/Program</t>
-  </si>
-  <si>
-    <t>Metabolic Bone Disease and Osteoporosis Center/ Osteoporosis and Metabolic Center</t>
-  </si>
-  <si>
-    <t>#2523 List of Terms 10-8-2021</t>
-  </si>
-  <si>
     <t>Skeletal Health Program</t>
   </si>
   <si>
-    <t>Bone Health Clinic/Center</t>
-  </si>
-  <si>
-    <t>Fracture Liaison Program/Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Own the Bone" </t>
+    <t>Bone Health Center</t>
+  </si>
+  <si>
+    <t>Bone Health Clinic</t>
+  </si>
+  <si>
+    <t>Osteoporosis Prevention Center</t>
+  </si>
+  <si>
+    <t>Osteoporosis Prevention Clinic</t>
+  </si>
+  <si>
+    <t>Osteoporosis Prevention Program</t>
+  </si>
+  <si>
+    <t>Osteoporosis and Metabolic Center</t>
+  </si>
+  <si>
+    <t>Metabolic Bone Disease Center</t>
+  </si>
+  <si>
+    <t>Secondary Fracture Prevention</t>
+  </si>
+  <si>
+    <t>Fracture Liaison</t>
+  </si>
+  <si>
+    <t>Fragility Fracture</t>
+  </si>
+  <si>
+    <t>Fracture Program</t>
+  </si>
+  <si>
+    <t>Fracture Center</t>
+  </si>
+  <si>
+    <t>Own the Bone</t>
+  </si>
+  <si>
+    <t>Healthy Bones Program</t>
+  </si>
+  <si>
+    <t>Capture the Fracture</t>
+  </si>
+  <si>
+    <t>Geriatric Fracture Care</t>
+  </si>
+  <si>
+    <t>Post Fracture Care Services</t>
+  </si>
+  <si>
+    <t>Orthogeriatric Service</t>
+  </si>
+  <si>
+    <t>Osteoporosis Liaison</t>
+  </si>
+  <si>
+    <t>Fracture Prevention Clinic</t>
+  </si>
+  <si>
+    <t>Fracture Prevention Service</t>
+  </si>
+  <si>
+    <t>Fracture Prevention Center</t>
+  </si>
+  <si>
+    <t>Orthopedic-Geriatric Co-Care Services</t>
+  </si>
+  <si>
+    <t>Orthopaedic-Geriatric Co-Care Services</t>
+  </si>
+  <si>
+    <t>Orthopaedic Orthopedic Geriatric Co Care Services</t>
+  </si>
+  <si>
+    <t>Orthopedic Geriatric Co Care Services</t>
+  </si>
+  <si>
+    <t>Orthopaedic Geriatric Co Care Services</t>
+  </si>
+  <si>
+    <t>SearchTerms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +169,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -265,6 +293,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -300,6 +345,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,46 +537,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -524,12 +589,12 @@
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -537,136 +602,175 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>